<commit_message>
added some more rows
</commit_message>
<xml_diff>
--- a/Data_Source_Exc.xlsx
+++ b/Data_Source_Exc.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Description</t>
   </si>
@@ -65,7 +65,73 @@
     <t>Date</t>
   </si>
   <si>
-    <t>my name is ali</t>
+    <t>UPI/KAZI SANA KAZI /078513505036/Payment from Ph</t>
+  </si>
+  <si>
+    <t>UPI-427637049656</t>
+  </si>
+  <si>
+    <t>- ₹30.00</t>
+  </si>
+  <si>
+    <t>₹2.72</t>
+  </si>
+  <si>
+    <t>UPI/KAZI SANA KAZI /344059039001/Payment from Ph</t>
+  </si>
+  <si>
+    <t>UPI-427620658857</t>
+  </si>
+  <si>
+    <t>- ₹10.00</t>
+  </si>
+  <si>
+    <t>₹32.72</t>
+  </si>
+  <si>
+    <t>UPI/Kazi Shoeboddin/395535689576/Payment from Ph</t>
+  </si>
+  <si>
+    <t>UPI-427376235606</t>
+  </si>
+  <si>
+    <t>- ₹34.00</t>
+  </si>
+  <si>
+    <t>₹117.72</t>
+  </si>
+  <si>
+    <t>UPI/Shaikh Mumtaz F/038147999834/Payment from Ph</t>
+  </si>
+  <si>
+    <t>UPI-427376185816</t>
+  </si>
+  <si>
+    <t>- ₹166.00</t>
+  </si>
+  <si>
+    <t>₹151.72</t>
+  </si>
+  <si>
+    <t>UPI/KaziShoeboddinM/463981491028/PaymentfromPhon</t>
+  </si>
+  <si>
+    <t>UPI-427375877465</t>
+  </si>
+  <si>
+    <t>₹200.00</t>
+  </si>
+  <si>
+    <t>₹317.72</t>
+  </si>
+  <si>
+    <t>UPI/KAZI SANA KAZI /322420393826/Payment from Ph</t>
+  </si>
+  <si>
+    <t>UPI-427264687389</t>
+  </si>
+  <si>
+    <t>- ₹50.00</t>
   </si>
 </sst>
 </file>
@@ -126,9 +192,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -141,9 +206,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -428,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -447,56 +509,150 @@
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="42.75">
-      <c r="A2" s="7">
-        <v>45566</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="6">
+        <v>45564</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="42.75">
-      <c r="A3" s="8">
+      <c r="A3" s="6">
         <v>45564</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="8">
-        <v>45565</v>
+    <row r="4" spans="1:5" ht="42.75">
+      <c r="A4" s="6">
+        <v>45567</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="42.75">
+      <c r="A5" s="6">
+        <v>45567</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="42.75">
+      <c r="A6" s="6">
+        <v>45564</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="42.75">
+      <c r="A7" s="6">
+        <v>45564</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="42.75">
+      <c r="A8" s="6">
+        <v>45564</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="42.75">
+      <c r="A9" s="6">
+        <v>45563</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed rows from the first column
</commit_message>
<xml_diff>
--- a/Data_Source_Exc.xlsx
+++ b/Data_Source_Exc.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Description</t>
   </si>
@@ -138,12 +138,6 @@
   </si>
   <si>
     <t>Flow</t>
-  </si>
-  <si>
-    <t>↗</t>
-  </si>
-  <si>
-    <t>↙</t>
   </si>
 </sst>
 </file>
@@ -184,7 +178,7 @@
       <name val="Roboto-medium"/>
     </font>
     <font>
-      <sz val="18"/>
+      <sz val="12"/>
       <color rgb="FF333333"/>
       <name val="Segoe UI"/>
       <family val="2"/>
@@ -511,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -542,9 +536,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="42.75">
-      <c r="A2" s="7" t="s">
-        <v>38</v>
-      </c>
+      <c r="A2" s="7"/>
       <c r="B2" s="6">
         <v>45564</v>
       </c>
@@ -562,9 +554,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="42.75">
-      <c r="A3" s="7" t="s">
-        <v>38</v>
-      </c>
+      <c r="A3" s="7"/>
       <c r="B3" s="6">
         <v>45564</v>
       </c>
@@ -582,9 +572,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="42.75">
-      <c r="A4" s="7" t="s">
-        <v>38</v>
-      </c>
+      <c r="A4" s="7"/>
       <c r="B4" s="6">
         <v>45567</v>
       </c>
@@ -602,9 +590,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="42.75">
-      <c r="A5" s="7" t="s">
-        <v>38</v>
-      </c>
+      <c r="A5" s="7"/>
       <c r="B5" s="6">
         <v>45567</v>
       </c>
@@ -622,9 +608,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="42.75">
-      <c r="A6" s="7" t="s">
-        <v>38</v>
-      </c>
+      <c r="A6" s="7"/>
       <c r="B6" s="6">
         <v>45564</v>
       </c>
@@ -642,9 +626,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="42.75">
-      <c r="A7" s="7" t="s">
-        <v>38</v>
-      </c>
+      <c r="A7" s="7"/>
       <c r="B7" s="6">
         <v>45564</v>
       </c>
@@ -662,9 +644,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="42.75">
-      <c r="A8" s="7" t="s">
-        <v>39</v>
-      </c>
+      <c r="A8" s="7"/>
       <c r="B8" s="6">
         <v>45564</v>
       </c>
@@ -682,9 +662,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="42.75">
-      <c r="A9" s="7" t="s">
-        <v>38</v>
-      </c>
+      <c r="A9" s="7"/>
       <c r="B9" s="6">
         <v>45563</v>
       </c>

</xml_diff>